<commit_message>
feat: added notes in Course 1 Module 2
</commit_message>
<xml_diff>
--- a/excel-basics/formula-functions/Monthly_Sales/Case Study - Monthly Sales Report.xlsx
+++ b/excel-basics/formula-functions/Monthly_Sales/Case Study - Monthly Sales Report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FAA7C0-76F6-40E3-A670-3BBDD706EE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116E3933-E1A9-4E5F-8D4C-099C09643325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{130225FD-24AD-4728-9152-74B9746A817F}"/>
   </bookViews>
@@ -176,11 +176,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -514,14 +514,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -1045,8 +1045,8 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1059,14 +1059,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -1548,7 +1548,7 @@
       <c r="B35" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="12">
         <f>SUM(C4:C33)</f>
         <v>115298</v>
       </c>
@@ -1557,7 +1557,7 @@
       <c r="B36" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="11">
         <f>SUM(C4:C33)</f>
         <v>115298</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="B37" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="11">
         <f>MIN(C4:C33)</f>
         <v>2560</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="B38" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="11">
         <f>MAX(C4:C33)</f>
         <v>4921</v>
       </c>
@@ -1610,6 +1610,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="15179a99-4cef-4bac-ab20-a4c03d7ec5db" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2aed4346-8012-4133-9837-e496d0f5c99a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EAC3B332A2FD04E918F9FD72E2B30AC" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5791f7a1e5ce60c682c7fd472657cfed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2aed4346-8012-4133-9837-e496d0f5c99a" xmlns:ns3="15179a99-4cef-4bac-ab20-a4c03d7ec5db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c4db72e02b896ab7bb9242ff846c9720" ns2:_="" ns3:_="">
     <xsd:import namespace="2aed4346-8012-4133-9837-e496d0f5c99a"/>
@@ -1826,27 +1846,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B55BE2C2-D947-480B-AEB2-F59EA82B4FEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="15179a99-4cef-4bac-ab20-a4c03d7ec5db"/>
+    <ds:schemaRef ds:uri="2aed4346-8012-4133-9837-e496d0f5c99a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="15179a99-4cef-4bac-ab20-a4c03d7ec5db" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2aed4346-8012-4133-9837-e496d0f5c99a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED0AB313-3178-48D8-8F17-381CEBFE5854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EEB051B-E50B-42A0-B0FB-A4FBD11C0758}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1863,23 +1882,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED0AB313-3178-48D8-8F17-381CEBFE5854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B55BE2C2-D947-480B-AEB2-F59EA82B4FEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="15179a99-4cef-4bac-ab20-a4c03d7ec5db"/>
-    <ds:schemaRef ds:uri="2aed4346-8012-4133-9837-e496d0f5c99a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>